<commit_message>
minor fixes op09 op10
</commit_message>
<xml_diff>
--- a/Relazione/Tabelle/TabelleAccessi.xlsx
+++ b/Relazione/Tabelle/TabelleAccessi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Basi_Di_Dati_2021\Relazione\Tabelle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756F7407-1AC3-4950-BCCF-728FFC07EBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC31F2-4A3E-43D5-A53D-AF218153A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{8B7D02E1-A157-41E1-83C1-B4728AF6E18B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$B$75:$E$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$B$81:$E$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="67">
   <si>
     <t>Concetto</t>
   </si>
@@ -433,7 +433,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: 1.000.002L x 1 all'anno = 1.000.002L all'anno = 1.000.002L all'anno</t>
+      <t>: 1.000.001L x 1 all'anno = 1.000.001L all'anno = 1.000.001L all'anno</t>
     </r>
   </si>
   <si>
@@ -456,7 +456,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: 50.002L x 1 all'anno = 50.002L all'anno = 50.002 all'anno</t>
+      <t>: 50.001L x 1 all'anno = 50.001L all'anno = 50.001 all'anno</t>
     </r>
   </si>
 </sst>
@@ -536,10 +536,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -856,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499E751A-00C8-4844-91DD-983FBD960ACD}">
-  <dimension ref="A2:G95"/>
+  <dimension ref="A2:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:E79"/>
+      <selection activeCell="B81" sqref="B81:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -908,23 +908,23 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B8" s="3" t="s">
@@ -1026,12 +1026,12 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
@@ -1101,12 +1101,12 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
@@ -1162,12 +1162,12 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
@@ -1321,12 +1321,12 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
@@ -1480,12 +1480,12 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
@@ -1583,12 +1583,12 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
@@ -1686,12 +1686,12 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
@@ -1734,12 +1734,12 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B77" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" s="4">
+        <v>5</v>
+      </c>
+      <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -1747,136 +1747,136 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B78" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B78" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B79" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="A80" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A81" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
+      <c r="B81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B82" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>3</v>
+      <c r="B82" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B83" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="4">
-        <v>1000000</v>
+        <v>1</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B84" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C84" s="2" t="s">
+      <c r="B84" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>59</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B88" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="4">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B89" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="4">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B85" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="4">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B86" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A88" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B89" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>3</v>
+      <c r="D89" s="4">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B90" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>5</v>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B91" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D91" s="4">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>9</v>
@@ -1904,61 +1904,35 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B92" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="4">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B93" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" s="4">
-        <v>60</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B94" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="4">
-        <v>60</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B95" s="8" t="s">
+      <c r="B93" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B84:E84"/>
     <mergeCell ref="B63:E63"/>
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="B54:E54"/>
@@ -1969,13 +1943,11 @@
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>